<commit_message>
some more c (useless tmp variables) deleted
</commit_message>
<xml_diff>
--- a/engineering-competition/dev_process.xlsx
+++ b/engineering-competition/dev_process.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Add Engineering Competition files</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>overview added in ---&gt;   gnuradio\engineering-competition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c86896c2d9ac90c9382981b8744282aafd76d861 </t>
+  </si>
+  <si>
+    <t>Divide et impera</t>
   </si>
 </sst>
 </file>
@@ -237,10 +243,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$C$2:$C$11</c:f>
+              <c:f>Tabelle1!$C$2:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>16321447886</c:v>
                 </c:pt>
@@ -270,6 +276,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>15967660563</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15868943608</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -530,10 +539,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$2:$B$11</c:f>
+              <c:f>Tabelle1!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1.43099646266E-6</c:v>
                 </c:pt>
@@ -563,6 +572,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1.4356257906900001E-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.26721215565E-6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2223,10 +2235,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2458,6 +2470,26 @@
         <v>24</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>159</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1.26721215565E-6</v>
+      </c>
+      <c r="C12">
+        <v>15868943608</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="1">
+        <v>42864</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
replacing the two loop with one containing modulu isn't that efficient...
</commit_message>
<xml_diff>
--- a/engineering-competition/dev_process.xlsx
+++ b/engineering-competition/dev_process.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Add Engineering Competition files</t>
   </si>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t>Divide et impera</t>
+  </si>
+  <si>
+    <t>4d722633c6f4821e59a9ca2b393870674f751c87</t>
+  </si>
+  <si>
+    <t>Last AVC Test for Today</t>
+  </si>
+  <si>
+    <t>63b114717e2642c74648886f53259cba73b21231</t>
+  </si>
+  <si>
+    <t>some more c (useless tmp variables) deleted</t>
   </si>
 </sst>
 </file>
@@ -243,10 +255,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$C$2:$C$12</c:f>
+              <c:f>Tabelle1!$C$2:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>16321447886</c:v>
                 </c:pt>
@@ -279,6 +291,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>15868943608</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15671770293</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15998233425</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -539,10 +557,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$2:$B$12</c:f>
+              <c:f>Tabelle1!$B$2:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1.43099646266E-6</c:v>
                 </c:pt>
@@ -574,6 +592,12 @@
                   <c:v>1.4356257906900001E-6</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>1.26721215565E-6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.26721215565E-6</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>1.26721215565E-6</c:v>
                 </c:pt>
               </c:numCache>
@@ -1866,15 +1890,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>78441</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>141194</xdr:rowOff>
+      <xdr:colOff>44823</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>29135</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2039470</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>26894</xdr:rowOff>
+      <xdr:colOff>2005852</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>105335</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1902,15 +1926,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2286000</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:colOff>2431677</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>40340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2487706</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:colOff>2633383</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>116540</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2235,10 +2259,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2490,6 +2514,46 @@
         <v>26</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>219</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1.26721215565E-6</v>
+      </c>
+      <c r="C13">
+        <v>15671770293</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="1">
+        <v>42869</v>
+      </c>
+      <c r="F13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>239</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1.26721215565E-6</v>
+      </c>
+      <c r="C14">
+        <v>15998233425</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="1">
+        <v>42870</v>
+      </c>
+      <c r="F14" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>